<commit_message>
Employee Management Test Cases Added
</commit_message>
<xml_diff>
--- a/TestData/LoginTestData.xlsx
+++ b/TestData/LoginTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PlaywrightFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C39FDC6-6496-4826-A260-76AFF7039576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8657C2CE-56DE-4D76-886B-DFABAF77BF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{787D8936-C9F3-4711-A0B4-310F3C385B62}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{787D8936-C9F3-4711-A0B4-310F3C385B62}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,16 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -441,7 +451,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>